<commit_message>
fix bugs and standard inputs/output
</commit_message>
<xml_diff>
--- a/docs/MOSFET_SELECTION.xlsx
+++ b/docs/MOSFET_SELECTION.xlsx
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/datasheet/2/408/TK13P25D_datasheet_en_20140106-1649876.pdf</t>
         </r>
@@ -44,6 +45,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPN70R600P7SATMA1?qs=HXFqYaX1Q2xIu5ZPZz84wg%3D%3D</t>
         </r>
@@ -56,6 +58,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/ProductDetail/Panjit/PJD18N20_L2_00001?qs=sPbYRqrBIVmlOEZjIPaS0Q%3D%3D</t>
         </r>
@@ -68,6 +71,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPD60R800CEAUMA1?qs=QIiuLP2W41AZ5k%2FyZxN%2Fzg%3D%3D</t>
         </r>
@@ -80,11 +84,25 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPD70R600P7SAUMA1?qs=KuGazDKa6A6CT0u%252Bhl2LvA%3D%3D</t>
         </r>
       </text>
     </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS-065-011-2-L-TR?qs=e8oIoAS2J1S2CQDrpAqVDA%3D%3D</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A8" authorId="0">
       <text>
         <r>
@@ -92,8 +110,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS-065-011-2-L-TR?qs=e8oIoAS2J1S2CQDrpAqVDA%3D%3D</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS-065-008-1-L-MR?qs=zW32dvEIR3u1kFOIdX8HEQ%3D%3D</t>
         </r>
       </text>
     </comment>
@@ -104,8 +123,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS-065-008-1-L-MR?qs=zW32dvEIR3u1kFOIdX8HEQ%3D%3D</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS66504B-MR?qs=OlC7AqGiEDmkLttA%2F6AlIA%3D%3D</t>
         </r>
       </text>
     </comment>
@@ -116,8 +136,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/GaN-Systems/GS66504B-MR?qs=OlC7AqGiEDmkLttA%2F6AlIA%3D%3D</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Wolfspeed/C2M0280120D?qs=8jfIC9vqKDvyc5TdTTxz8A%3D%3D</t>
         </r>
       </text>
     </comment>
@@ -128,8 +149,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Wolfspeed/C2M0280120D?qs=8jfIC9vqKDvyc5TdTTxz8A%3D%3D</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Siliconix/IRF640PBF-BE3?qs=7MVldsJ5Uaw%2FQaSyVtWN8A%3D%3D</t>
         </r>
       </text>
     </comment>
@@ -140,92 +162,165 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Toshiba/TPN2010FNHL1Q?qs=2kOmHSv6VfTUScjGDcny4Q%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXTH220N20X4?qs=IS%252B4QmGtzzo%252BEf2yYdkgiw%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXTT220N20X4HV?qs=IS%252B4QmGtzzolLLv7Nw%2FWsw%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXFK240N25X3?qs=BZBei1rCqCAj%252BBdeJke%2F8g%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPP110N20NA?qs=oPPfIaWL1l22VVnyZkYisw%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXFT140N20X3HV?qs=uwxL4vQweFMNd0PZCXS7bg%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPB107N20N3-G?qs=mzcOS1kGbgdtYi4qUqxC7Q%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/BSZ900N20NS3-G?qs=HwMeRNENlMa4%252BZeQQWvG8w%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPT60R125CFD7XTMA1?qs=sPbYRqrBIVkrhpzeglBnDA%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Wolfspeed/C3M0280090D?qs=nxZbHzLpdvfcUe1hs5VeOQ%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Siliconix/SQD10950E_GE3?qs=%252B6g0mu59x7JO%2FIaFyGY9oQ%3D%3D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Siliconix/IRF640PBF-BE3?qs=7MVldsJ5Uaw%2FQaSyVtWN8A%3D%3D</t>
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Toshiba/TPN2010FNHL1Q?qs=2kOmHSv6VfTUScjGDcny4Q%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXTH220N20X4?qs=IS%252B4QmGtzzo%252BEf2yYdkgiw%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXTT220N20X4HV?qs=IS%252B4QmGtzzolLLv7Nw%2FWsw%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A17" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXFK240N25X3?qs=BZBei1rCqCAj%252BBdeJke%2F8g%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPP110N20NA?qs=oPPfIaWL1l22VVnyZkYisw%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/IXYS/IXFT140N20X3HV?qs=uwxL4vQweFMNd0PZCXS7bg%3D%3D</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-Technologies/IPB107N20N3-G?qs=mzcOS1kGbgdtYi4qUqxC7Q%3D%3D</t>
+    <comment ref="A26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Siliconix/SIHP10N40D-GE3?qs=CJFgc%252B3p06iiWRia4DrQlg%3D%3D</t>
         </r>
       </text>
     </comment>
@@ -234,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t xml:space="preserve">Component Part</t>
   </si>
@@ -348,6 +443,36 @@
   </si>
   <si>
     <t xml:space="preserve">TO-263-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF200P222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSZ900N20NS3 G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSDSON-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPT60R125CFD7XTMA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSOF-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3M0280090D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQD10950E_GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIHH186N60EF-T1GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerPAK 8 x 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIHP10N40D-GE3</t>
   </si>
 </sst>
 </file>
@@ -363,6 +488,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -383,14 +509,21 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -427,16 +560,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,6 +622,81 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -457,530 +705,682 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="16.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <f aca="false">80*10^-12</f>
         <v>8E-011</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <f aca="false">F2*E2</f>
         <v>3.28E-011</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <f aca="false">10*10^-12</f>
         <v>1E-011</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">F3*E3</f>
         <v>1E-011</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <f aca="false">125*10^-3*2</f>
         <v>0.25</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <f aca="false">100*10^-12</f>
         <v>1E-010</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <f aca="false">F4*E4</f>
         <v>2.5E-011</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1.01</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>5.5</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">35*10^-12</f>
         <v>3.5E-011</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">F5*E5</f>
         <v>5.6E-011</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" s="6" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="4" t="n">
         <v>1.06</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="4" t="n">
         <v>8.5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.95</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="5" t="n">
         <f aca="false">10*10^-12</f>
         <v>1E-011</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="5" t="n">
         <f aca="false">F6*E6</f>
         <v>9.5E-012</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="0" t="n">
-        <f aca="false">F7*E7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>4.75</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.32</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <f aca="false">75*10^-12</f>
         <v>7.5E-011</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">F8*E8</f>
+      <c r="G7" s="1" t="n">
+        <f aca="false">F7*E7</f>
         <v>2.4E-011</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="8" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3.55</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">55*10^-12</f>
         <v>5.5E-011</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">F9*E9</f>
+      <c r="G8" s="1" t="n">
+        <f aca="false">F8*E8</f>
         <v>3.41E-011</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>13.86</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.26</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <f aca="false">80*10^-12</f>
         <v>8E-011</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">F10*E10</f>
+      <c r="G9" s="1" t="n">
+        <f aca="false">F9*E9</f>
         <v>2.08E-011</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>9.04</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <f aca="false">0.55</f>
         <v>0.55</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <f aca="false">60*10^-12</f>
         <v>6E-011</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">F11*E11</f>
+      <c r="G10" s="1" t="n">
+        <f aca="false">F10*E10</f>
         <v>3.3E-011</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>2.83</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <f aca="false">0.18</f>
         <v>0.18</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <f aca="false">225*10^-12</f>
         <v>2.25E-010</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">F12*E12</f>
+      <c r="G11" s="1" t="n">
+        <f aca="false">F11*E11</f>
         <v>4.05E-011</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1.55</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <f aca="false">0.375</f>
         <v>0.375</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <f aca="false">50*10^-12</f>
         <v>5E-011</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">F13*E13</f>
+      <c r="G12" s="1" t="n">
+        <f aca="false">F12*E12</f>
         <v>1.875E-011</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="0" t="n">
-        <f aca="false">F14*E14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>19.26</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <f aca="false">0.015</f>
         <v>0.015</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <f aca="false">700*10^-12</f>
         <v>7E-010</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">F15*E15</f>
+      <c r="G13" s="1" t="n">
+        <f aca="false">F13*E13</f>
         <v>1.05E-011</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+    <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>20.61</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>0.015</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F14" s="7" t="n">
         <f aca="false">700*10^-12</f>
         <v>7E-010</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">F16*E16</f>
+      <c r="G14" s="1" t="n">
+        <f aca="false">F14*E14</f>
         <v>1.05E-011</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>34.72</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.015</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <f aca="false">1050*10^-12</f>
         <v>1.05E-009</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">F17*E17</f>
+      <c r="G15" s="1" t="n">
+        <f aca="false">F15*E15</f>
         <v>1.575E-011</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="16" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>11.2</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <f aca="false">0.04</f>
         <v>0.04</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <f aca="false">450*10^-12</f>
         <v>4.5E-010</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">F18*E18</f>
+      <c r="G16" s="1" t="n">
+        <f aca="false">F16*E16</f>
         <v>1.8E-011</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="17" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>15.8</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <f aca="false">500*10^-12</f>
         <v>5E-010</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">F19*E19</f>
+      <c r="G17" s="1" t="n">
+        <f aca="false">F17*E17</f>
         <v>1E-011</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="18" s="6" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B18" s="4" t="n">
         <v>9.34</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C18" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="F20" s="0" t="n">
+      <c r="E18" s="4" t="n">
+        <f aca="false">9*10^-3*2</f>
+        <v>0.018</v>
+      </c>
+      <c r="F18" s="5" t="n">
         <f aca="false">450*10^-12</f>
         <v>4.5E-010</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G18" s="5" t="n">
+        <f aca="false">F18*E18</f>
+        <v>8.1E-012</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>11.28</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">556/8</f>
+        <v>69.5</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">900*10^-12</f>
+        <v>9E-010</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">F19*E19</f>
+        <v>9E-012</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">55*10^-12</f>
+        <v>5.5E-011</v>
+      </c>
+      <c r="G20" s="1" t="n">
         <f aca="false">F20*E20</f>
-        <v>9E-012</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G21" s="0" t="n">
+        <v>8.8E-012</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">0.195</f>
+        <v>0.195</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">45*10^-12</f>
+        <v>4.5E-011</v>
+      </c>
+      <c r="G21" s="1" t="n">
         <f aca="false">F21*E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G22" s="0" t="n">
+        <v>8.775E-012</v>
+      </c>
+    </row>
+    <row r="22" s="12" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <f aca="false">0.3*1.18</f>
+        <v>0.354</v>
+      </c>
+      <c r="F22" s="11" t="n">
+        <f aca="false">55*10^-12</f>
+        <v>5.5E-011</v>
+      </c>
+      <c r="G22" s="11" t="n">
         <f aca="false">F22*E22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="0" t="n">
+        <v>1.947E-011</v>
+      </c>
+    </row>
+    <row r="23" s="12" customFormat="true" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <f aca="false">0.13*2.15</f>
+        <v>0.2795</v>
+      </c>
+      <c r="F23" s="11" t="n">
+        <f aca="false">60*10^-12</f>
+        <v>6E-011</v>
+      </c>
+      <c r="G23" s="11" t="n">
         <f aca="false">F23*E23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="0" t="n">
+        <v>1.677E-011</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">114/8</f>
+        <v>14.25</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">0.168*2.1</f>
+        <v>0.3528</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">60*10^-12</f>
+        <v>6E-011</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <f aca="false">F24*E24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="0" t="n">
+        <v>2.1168E-011</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">125/8</f>
+        <v>15.625</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">0.18*2*0.85</f>
+        <v>0.306</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">200*10^-12</f>
+        <v>2E-010</v>
+      </c>
+      <c r="G25" s="1" t="n">
         <f aca="false">F25*E25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="0" t="n">
+        <v>6.12E-011</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">147/8</f>
+        <v>18.375</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <f aca="false">0.5*2</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">60*10^-12</f>
+        <v>6E-011</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <f aca="false">F26*E26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G27" s="0" t="n">
-        <f aca="false">F27*E27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="0" t="n">
-        <f aca="false">F28*E28</f>
-        <v>0</v>
+        <v>6E-011</v>
       </c>
     </row>
   </sheetData>
@@ -996,6 +1396,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00A933"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A1048576 A1:A20">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>